<commit_message>
fix name import file, chanfe file.xlsx
</commit_message>
<xml_diff>
--- a/public/product/product-stock-template.xlsx
+++ b/public/product/product-stock-template.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PIPI_LOL\Downloads\Telegram Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mayling\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F84E5374-E5A3-49AB-94DD-B02AFB4363EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,25 +28,25 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Nombre</t>
-  </si>
-  <si>
     <t>Código</t>
   </si>
   <si>
     <t>Área</t>
   </si>
   <si>
-    <t>Cantidad</t>
+    <t>Causa</t>
   </si>
   <si>
-    <t>Causa</t>
+    <t>Producto</t>
+  </si>
+  <si>
+    <t>Disponibilidad</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -431,11 +430,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
@@ -443,7 +442,7 @@
     <col min="1" max="1" width="26.25" style="2" customWidth="1"/>
     <col min="2" max="2" width="21.25" style="2" customWidth="1"/>
     <col min="3" max="3" width="17.75" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9.75" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.25" style="2" customWidth="1"/>
     <col min="6" max="1022" width="8.625" style="2"/>
     <col min="1023" max="1024" width="10.375" style="2" customWidth="1"/>
@@ -452,19 +451,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="38.85" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18.600000000000001" customHeight="1"/>
@@ -484,7 +483,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
@@ -497,7 +496,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>

</xml_diff>